<commit_message>
Refactored files, changed vector size back to 128
</commit_message>
<xml_diff>
--- a/Performance_testing.xlsx
+++ b/Performance_testing.xlsx
@@ -206,6 +206,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -225,15 +234,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -700,7 +700,7 @@
   <dimension ref="B1:N22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -720,26 +720,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
     </row>
     <row r="2" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
@@ -747,66 +747,66 @@
     <row r="3" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
-      <c r="K3" s="13"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="16"/>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
       <c r="N3" s="2"/>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="13"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="16"/>
+      <c r="K4" s="16"/>
       <c r="L4" s="4"/>
       <c r="M4" s="4"/>
       <c r="N4" s="2"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="16"/>
+      <c r="K5" s="16"/>
       <c r="L5" s="5"/>
       <c r="M5" s="4"/>
       <c r="N5" s="2"/>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="13"/>
-      <c r="K6" s="13"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="16"/>
       <c r="L6" s="5"/>
       <c r="M6" s="4"/>
       <c r="N6" s="2"/>
     </row>
-    <row r="7" spans="2:14" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="14"/>
+    <row r="7" spans="2:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="17"/>
+      <c r="J7" s="17"/>
+      <c r="K7" s="17"/>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
@@ -844,7 +844,7 @@
       </c>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B9" s="16">
+      <c r="B9" s="9">
         <v>50000</v>
       </c>
       <c r="C9" s="8">
@@ -864,7 +864,7 @@
       </c>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B10" s="18"/>
+      <c r="B10" s="11"/>
       <c r="C10" s="6">
         <v>10</v>
       </c>
@@ -882,7 +882,7 @@
       </c>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B11" s="17"/>
+      <c r="B11" s="10"/>
       <c r="C11" s="6">
         <v>50</v>
       </c>
@@ -914,7 +914,7 @@
       <c r="K12" s="1"/>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B13" s="16">
+      <c r="B13" s="9">
         <v>1000000</v>
       </c>
       <c r="C13" s="1">
@@ -934,7 +934,7 @@
       <c r="K13" s="1"/>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B14" s="17"/>
+      <c r="B14" s="10"/>
       <c r="C14" s="1">
         <v>50</v>
       </c>
@@ -954,32 +954,32 @@
     <row r="15" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
-      <c r="D15" s="9" t="s">
+      <c r="D15" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="E15" s="9"/>
-      <c r="F15" s="10" t="s">
+      <c r="E15" s="12"/>
+      <c r="F15" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="G15" s="11"/>
-      <c r="H15" s="15"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="10"/>
-      <c r="K15" s="11"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="18"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="14"/>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="D16" s="12" t="s">
+      <c r="D16" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12" t="s">
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="I16" s="12"/>
-      <c r="J16" s="12"/>
-      <c r="K16" s="12"/>
+      <c r="I16" s="15"/>
+      <c r="J16" s="15"/>
+      <c r="K16" s="15"/>
     </row>
     <row r="22" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G22" t="s">
@@ -988,17 +988,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="B9:B11"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="D16:G16"/>
     <mergeCell ref="H1:I7"/>
     <mergeCell ref="J1:K7"/>
     <mergeCell ref="H16:K16"/>
     <mergeCell ref="H15:K15"/>
     <mergeCell ref="D1:E7"/>
     <mergeCell ref="F1:G7"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="D16:G16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>